<commit_message>
updated sheets and created utils file
</commit_message>
<xml_diff>
--- a/sheets/datasets.xlsx
+++ b/sheets/datasets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauth\OneDrive\Desktop\LLM Assistant File - V2\fine_tuning\embeddings\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39744944-763A-4B50-917B-59E71F78BBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E0B696-ECEF-42AA-801D-0AABCB3AD955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,26 @@
     <sheet name="keywords" sheetId="1" r:id="rId1"/>
     <sheet name="sub_queries" sheetId="2" r:id="rId2"/>
     <sheet name="chunks" sheetId="3" r:id="rId3"/>
-    <sheet name="openia" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="266">
   <si>
     <t>measurement system</t>
   </si>
@@ -967,474 +979,6 @@
   </si>
   <si>
     <t>This text talks about uncertainty, which measures the potential error or margin of error in measurements. It explains two types: uncertainty of magnitudes (specific variables like temperature or pressure) and uncertainty of the measurement system (overall flow measurement), with both types stored separately in the database.</t>
-  </si>
-  <si>
-    <t>provider</t>
-  </si>
-  <si>
-    <t>What are the columns in the pressure_data table?</t>
-  </si>
-  <si>
-    <t>openai</t>
-  </si>
-  <si>
-    <t>What is the data type of the uncertainty_value column?</t>
-  </si>
-  <si>
-    <t>What is the format of the timestamp column?</t>
-  </si>
-  <si>
-    <t>Are there any indexes on the pressure_data table?</t>
-  </si>
-  <si>
-    <t>What are the common tags used in the pressure_data table?</t>
-  </si>
-  <si>
-    <t>How is the uncertainty_value calculated or derived?</t>
-  </si>
-  <si>
-    <t>Are there any constraints on the pressure_data table?</t>
-  </si>
-  <si>
-    <t>What tables are related to calibration points?</t>
-  </si>
-  <si>
-    <t>What columns are present in the calibration points table?</t>
-  </si>
-  <si>
-    <t>How is the calibration number stored in the database?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between calibration points and other tables?</t>
-  </si>
-  <si>
-    <t>What is the data type of the calibration number?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions commonly used with calibration points?</t>
-  </si>
-  <si>
-    <t>What is the typical structure of a query retrieving calibration points?</t>
-  </si>
-  <si>
-    <t>What are the main tables related to pressure data?</t>
-  </si>
-  <si>
-    <t>What columns exist in the pressure_data table?</t>
-  </si>
-  <si>
-    <t>Are there any constraints on the calibration number field?</t>
-  </si>
-  <si>
-    <t>What is the typical query structure to retrieve calibration points?</t>
-  </si>
-  <si>
-    <t>What columns are available in the equipment table?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between equipment and calibration points?</t>
-  </si>
-  <si>
-    <t>What is the data type of the equipment tag?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions typically used for retrieving calibration points?</t>
-  </si>
-  <si>
-    <t>What are the columns in the equipment table?</t>
-  </si>
-  <si>
-    <t>What are the columns in the equipment_type table?</t>
-  </si>
-  <si>
-    <t>What are the columns in the equipment_classification table?</t>
-  </si>
-  <si>
-    <t>What are the relationships between equipment and equipment_type?</t>
-  </si>
-  <si>
-    <t>What are the relationships between equipment and equipment_classification?</t>
-  </si>
-  <si>
-    <t>What is the data type of the tag column in the equipment table?</t>
-  </si>
-  <si>
-    <t>Are there any constraints on the tag column in the equipment table?</t>
-  </si>
-  <si>
-    <t>What tables contain information about equipment classes?</t>
-  </si>
-  <si>
-    <t>What fields are available in the equipment table?</t>
-  </si>
-  <si>
-    <t>How is the equipment type linked to the equipment tag?</t>
-  </si>
-  <si>
-    <t>What is the relationship between equipment and systems?</t>
-  </si>
-  <si>
-    <t>Are there any specific filters for secondary equipment?</t>
-  </si>
-  <si>
-    <t>What is the structure of the system table?</t>
-  </si>
-  <si>
-    <t>How are serial numbers stored in the database?</t>
-  </si>
-  <si>
-    <t>What tables store equipment information?</t>
-  </si>
-  <si>
-    <t>What columns are present in the equipment table?</t>
-  </si>
-  <si>
-    <t>How is calibration data related to equipment?</t>
-  </si>
-  <si>
-    <t>What is the data type of the calibration date column?</t>
-  </si>
-  <si>
-    <t>Are there any constraints on the calibration date?</t>
-  </si>
-  <si>
-    <t>How can I filter calibration records by equipment tag?</t>
-  </si>
-  <si>
-    <t>What tables contain information about equipment serials?</t>
-  </si>
-  <si>
-    <t>What variables can each equipment read?</t>
-  </si>
-  <si>
-    <t>How is the tag &amp;&amp;&amp;EMED-3138.11-128&amp;&amp;&amp; related to equipment?</t>
-  </si>
-  <si>
-    <t>What is the relationship between equipment and their serials?</t>
-  </si>
-  <si>
-    <t>Are there any specific attributes associated with the tag &amp;&amp;&amp;EMED-3138.11-128&amp;&amp;&amp;?</t>
-  </si>
-  <si>
-    <t>What is the structure of the data related to equipment in the database?</t>
-  </si>
-  <si>
-    <t>Are there any constraints or filters related to the equipment data?</t>
-  </si>
-  <si>
-    <t>What tables store uncertainty reports?</t>
-  </si>
-  <si>
-    <t>What columns are present in the uncertainty reports table?</t>
-  </si>
-  <si>
-    <t>How is temperature data related to equipment tags?</t>
-  </si>
-  <si>
-    <t>How can I filter uncertainty reports by equipment tag?</t>
-  </si>
-  <si>
-    <t>What is the format of the date column in the uncertainty reports?</t>
-  </si>
-  <si>
-    <t>How can I retrieve the latest report for a specific equipment tag?</t>
-  </si>
-  <si>
-    <t>What columns are available in the uncertainty reports table?</t>
-  </si>
-  <si>
-    <t>How is temperature recorded in the database?</t>
-  </si>
-  <si>
-    <t>How is differential pressure recorded in the database?</t>
-  </si>
-  <si>
-    <t>What is the relationship between tags and uncertainty reports?</t>
-  </si>
-  <si>
-    <t>How can I filter reports by the tag EMED-3138.12-050?</t>
-  </si>
-  <si>
-    <t>What is the structure of the latest reports in the database?</t>
-  </si>
-  <si>
-    <t>What are the columns in the uncertainty_reports table?</t>
-  </si>
-  <si>
-    <t>What is the data type of the report_date column?</t>
-  </si>
-  <si>
-    <t>How is the equipment_tag column structured?</t>
-  </si>
-  <si>
-    <t>Are there any indexes on the uncertainty_reports table?</t>
-  </si>
-  <si>
-    <t>What is the typical format of report_details?</t>
-  </si>
-  <si>
-    <t>Are there any constraints on the equipment_tag column?</t>
-  </si>
-  <si>
-    <t>What is the most recent report_date for equipment with tag EMED-3138.12-050-DPT?</t>
-  </si>
-  <si>
-    <t>How is temperature data stored in the database?</t>
-  </si>
-  <si>
-    <t>What is the structure of the tag EMED-3138.12-050?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between uncertainty reports and temperature data?</t>
-  </si>
-  <si>
-    <t>How can I filter uncertainty reports by tag?</t>
-  </si>
-  <si>
-    <t>What is the format of the last report retrieval?</t>
-  </si>
-  <si>
-    <t>How is the calibration number structured in the database?</t>
-  </si>
-  <si>
-    <t>Are there any foreign keys related to calibration points?</t>
-  </si>
-  <si>
-    <t>What is the relationship between calibration points and calibrations?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions commonly used with calibration queries?</t>
-  </si>
-  <si>
-    <t>What tables are related to flow computers?</t>
-  </si>
-  <si>
-    <t>What columns are available in the flow computers table?</t>
-  </si>
-  <si>
-    <t>What tables are related to meter streams?</t>
-  </si>
-  <si>
-    <t>What columns are available in the meter streams table?</t>
-  </si>
-  <si>
-    <t>How are flow computers and meter streams linked?</t>
-  </si>
-  <si>
-    <t>What is the data type of the tags in the flow computers table?</t>
-  </si>
-  <si>
-    <t>What is the data type of the meter streams in the meter streams table?</t>
-  </si>
-  <si>
-    <t>What columns are present in the flow computers table?</t>
-  </si>
-  <si>
-    <t>What is the structure of the measurement systems table?</t>
-  </si>
-  <si>
-    <t>What defines a flowboss in the database?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between system tags and flow computers?</t>
-  </si>
-  <si>
-    <t>What other relevant tags are associated with flow computers?</t>
-  </si>
-  <si>
-    <t>What is the relationship between flow computers and measurement systems?</t>
-  </si>
-  <si>
-    <t>What columns are available in the measurement systems table?</t>
-  </si>
-  <si>
-    <t>Are there any tags associated with flow computers?</t>
-  </si>
-  <si>
-    <t>What is the structure of the data related to computer types?</t>
-  </si>
-  <si>
-    <t>What tables contain information about computers?</t>
-  </si>
-  <si>
-    <t>What columns are available in the computer table?</t>
-  </si>
-  <si>
-    <t>How are computers associated with measurement systems?</t>
-  </si>
-  <si>
-    <t>What is the structure of the measurement system table?</t>
-  </si>
-  <si>
-    <t>What columns are available for system tags?</t>
-  </si>
-  <si>
-    <t>What columns are available for computer tags?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between system tags and computers?</t>
-  </si>
-  <si>
-    <t>What are the columns in the computer_reports table?</t>
-  </si>
-  <si>
-    <t>What type of data is stored in the tag column?</t>
-  </si>
-  <si>
-    <t>What type of data is stored in the report_date column?</t>
-  </si>
-  <si>
-    <t>What type of data is stored in the details column?</t>
-  </si>
-  <si>
-    <t>Are there any constraints or indexes on the computer_reports table?</t>
-  </si>
-  <si>
-    <t>How is the report_date formatted in the database?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between computer_reports and other tables?</t>
-  </si>
-  <si>
-    <t>What columns are available in the table related to computer tags?</t>
-  </si>
-  <si>
-    <t>Is there a table that logs daily reports for computer tags?</t>
-  </si>
-  <si>
-    <t>What is the structure of the daily report table?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions for the computer tag FQI-EMED-3138.12-050?</t>
-  </si>
-  <si>
-    <t>What date formats are used in the database?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between the computer tag table and other tables?</t>
-  </si>
-  <si>
-    <t>What tables contain usage statistics for computers?</t>
-  </si>
-  <si>
-    <t>What columns are available in the usage statistics tables?</t>
-  </si>
-  <si>
-    <t>Is there a specific table for daily usage statistics?</t>
-  </si>
-  <si>
-    <t>What is the format of the date column in the usage statistics table?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions needed for the computer tag FQI-EMED-3138.12-050?</t>
-  </si>
-  <si>
-    <t>What is the relationship between the computer tags and usage statistics?</t>
-  </si>
-  <si>
-    <t>Are there any existing reports for daily usage statistics?</t>
-  </si>
-  <si>
-    <t>What tables contain report information?</t>
-  </si>
-  <si>
-    <t>What is the structure of the report table?</t>
-  </si>
-  <si>
-    <t>What columns are available in the report table?</t>
-  </si>
-  <si>
-    <t>How are reports associated with computer tags?</t>
-  </si>
-  <si>
-    <t>What is the format of the computer tag in the database?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions for retrieving the latest report?</t>
-  </si>
-  <si>
-    <t>What is the date format used for report dates?</t>
-  </si>
-  <si>
-    <t>Is there a specific table for daily reports?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between the computer tags and daily reports?</t>
-  </si>
-  <si>
-    <t>What filters can be applied to retrieve data for a specific date?</t>
-  </si>
-  <si>
-    <t>What additional information is relevant for the computer tag FQI-EMED-3138.12-050?</t>
-  </si>
-  <si>
-    <t>What columns are available in the uncertainty results table?</t>
-  </si>
-  <si>
-    <t>How is the tag EMED-3102-02-010 related to uncertainty results?</t>
-  </si>
-  <si>
-    <t>What is the data type of the tag column?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions typically applied to retrieve uncertainty results?</t>
-  </si>
-  <si>
-    <t>What is the structure of the most recent uncertainty result?</t>
-  </si>
-  <si>
-    <t>Are there any indexes on the uncertainty results table that could optimize the query?</t>
-  </si>
-  <si>
-    <t>How is uncertainty data related to measurement systems?</t>
-  </si>
-  <si>
-    <t>What is the structure of the uncertainty results table?</t>
-  </si>
-  <si>
-    <t>Are there any filters or conditions for retrieving uncertainty results?</t>
-  </si>
-  <si>
-    <t>Is there a specific way to query by measurement system tags?</t>
-  </si>
-  <si>
-    <t>What tables contain information about flow rate uncertainty?</t>
-  </si>
-  <si>
-    <t>What columns are available in the table related to curve_OF_UNCERTAINTY?</t>
-  </si>
-  <si>
-    <t>How is the certificate number EMED-010-1 stored in the database?</t>
-  </si>
-  <si>
-    <t>Are there any relationships between flow rate uncertainty and certificate numbers?</t>
-  </si>
-  <si>
-    <t>What is the data type of the flow rate uncertainty fingerprint points?</t>
-  </si>
-  <si>
-    <t>Are there any specific filters or conditions needed to retrieve the uncertainty points?</t>
-  </si>
-  <si>
-    <t>What is the structure of the data returned for flow rate uncertainty?</t>
-  </si>
-  <si>
-    <t>What columns are available in the table for measurement system EMED-3102-02-010?</t>
-  </si>
-  <si>
-    <t>How is the date stored in the database for measurements?</t>
-  </si>
-  <si>
-    <t>What is the data type of static pressure in the measurement system?</t>
-  </si>
-  <si>
-    <t>What is the data type of differential pressure in the measurement system?</t>
-  </si>
-  <si>
-    <t>What is the data type of temperature in the measurement system?</t>
-  </si>
-  <si>
-    <t>What is the data type of flow rate volume in the measurement system?</t>
   </si>
   <si>
     <t>This text talks about equipment calibration, a process that ensures measurement accuracy by correcting deviations. Calibration is performed periodically with two main cycles: as-found (pre-adjustment) and as-left (post-adjustment), and includes uncertainty of the magnitude, which affects the margin of error in measurements.</t>
@@ -1772,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:A177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A151" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -2670,15 +2214,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D188"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A180" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="78.5546875" customWidth="1"/>
+    <col min="1" max="1" width="82.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="54.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4761,13 +4305,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C6AAD4-06B0-442F-8B22-9E2FEAE61891}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="40.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="54.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.88671875" style="2" customWidth="1"/>
@@ -4897,7 +4441,7 @@
         <v>233</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>421</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4919,1543 +4463,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011D4B6-3E39-49FF-9C56-25E7030DB4DD}">
-  <dimension ref="A1:B190"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="62.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>269</v>
-      </c>
-      <c r="B4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>271</v>
-      </c>
-      <c r="B6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>274</v>
-      </c>
-      <c r="B9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B11" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B12" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>278</v>
-      </c>
-      <c r="B13" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>279</v>
-      </c>
-      <c r="B14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>280</v>
-      </c>
-      <c r="B15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>281</v>
-      </c>
-      <c r="B16" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>282</v>
-      </c>
-      <c r="B17" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>268</v>
-      </c>
-      <c r="B18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>269</v>
-      </c>
-      <c r="B19" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>270</v>
-      </c>
-      <c r="B20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>271</v>
-      </c>
-      <c r="B21" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>272</v>
-      </c>
-      <c r="B22" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>274</v>
-      </c>
-      <c r="B23" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>275</v>
-      </c>
-      <c r="B24" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>276</v>
-      </c>
-      <c r="B25" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B26" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>278</v>
-      </c>
-      <c r="B27" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>283</v>
-      </c>
-      <c r="B28" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>284</v>
-      </c>
-      <c r="B29" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>181</v>
-      </c>
-      <c r="B30" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>203</v>
-      </c>
-      <c r="B32" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>285</v>
-      </c>
-      <c r="B33" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>286</v>
-      </c>
-      <c r="B34" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>287</v>
-      </c>
-      <c r="B35" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>288</v>
-      </c>
-      <c r="B36" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>289</v>
-      </c>
-      <c r="B37" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>290</v>
-      </c>
-      <c r="B38" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>291</v>
-      </c>
-      <c r="B39" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>292</v>
-      </c>
-      <c r="B40" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>293</v>
-      </c>
-      <c r="B41" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>294</v>
-      </c>
-      <c r="B42" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>295</v>
-      </c>
-      <c r="B43" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>296</v>
-      </c>
-      <c r="B44" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>297</v>
-      </c>
-      <c r="B45" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>298</v>
-      </c>
-      <c r="B46" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>299</v>
-      </c>
-      <c r="B47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>300</v>
-      </c>
-      <c r="B48" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>301</v>
-      </c>
-      <c r="B49" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>302</v>
-      </c>
-      <c r="B50" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>303</v>
-      </c>
-      <c r="B51" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>304</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>305</v>
-      </c>
-      <c r="B53" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>306</v>
-      </c>
-      <c r="B55" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>307</v>
-      </c>
-      <c r="B56" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>308</v>
-      </c>
-      <c r="B57" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B58" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>310</v>
-      </c>
-      <c r="B59" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>311</v>
-      </c>
-      <c r="B60" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>312</v>
-      </c>
-      <c r="B61" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>313</v>
-      </c>
-      <c r="B62" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>314</v>
-      </c>
-      <c r="B63" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>315</v>
-      </c>
-      <c r="B64" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>316</v>
-      </c>
-      <c r="B65" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>317</v>
-      </c>
-      <c r="B66" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>318</v>
-      </c>
-      <c r="B67" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>88</v>
-      </c>
-      <c r="B68" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>319</v>
-      </c>
-      <c r="B69" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>320</v>
-      </c>
-      <c r="B70" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>321</v>
-      </c>
-      <c r="B71" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>316</v>
-      </c>
-      <c r="B72" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>322</v>
-      </c>
-      <c r="B73" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>323</v>
-      </c>
-      <c r="B74" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>324</v>
-      </c>
-      <c r="B75" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>325</v>
-      </c>
-      <c r="B76" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>326</v>
-      </c>
-      <c r="B77" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>327</v>
-      </c>
-      <c r="B78" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>328</v>
-      </c>
-      <c r="B79" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>329</v>
-      </c>
-      <c r="B80" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>330</v>
-      </c>
-      <c r="B81" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>331</v>
-      </c>
-      <c r="B82" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>332</v>
-      </c>
-      <c r="B83" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>333</v>
-      </c>
-      <c r="B84" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>334</v>
-      </c>
-      <c r="B85" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>316</v>
-      </c>
-      <c r="B86" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>317</v>
-      </c>
-      <c r="B87" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>335</v>
-      </c>
-      <c r="B88" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>336</v>
-      </c>
-      <c r="B89" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>337</v>
-      </c>
-      <c r="B90" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>338</v>
-      </c>
-      <c r="B91" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>339</v>
-      </c>
-      <c r="B92" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>274</v>
-      </c>
-      <c r="B93" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>215</v>
-      </c>
-      <c r="B94" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>340</v>
-      </c>
-      <c r="B95" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>341</v>
-      </c>
-      <c r="B96" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>342</v>
-      </c>
-      <c r="B97" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>343</v>
-      </c>
-      <c r="B98" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>278</v>
-      </c>
-      <c r="B99" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>344</v>
-      </c>
-      <c r="B100" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>345</v>
-      </c>
-      <c r="B101" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>346</v>
-      </c>
-      <c r="B102" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>347</v>
-      </c>
-      <c r="B103" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>348</v>
-      </c>
-      <c r="B104" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>349</v>
-      </c>
-      <c r="B105" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>350</v>
-      </c>
-      <c r="B106" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>136</v>
-      </c>
-      <c r="B107" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>351</v>
-      </c>
-      <c r="B108" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>219</v>
-      </c>
-      <c r="B109" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>352</v>
-      </c>
-      <c r="B110" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>353</v>
-      </c>
-      <c r="B111" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>354</v>
-      </c>
-      <c r="B112" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>355</v>
-      </c>
-      <c r="B113" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>136</v>
-      </c>
-      <c r="B114" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>345</v>
-      </c>
-      <c r="B115" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>356</v>
-      </c>
-      <c r="B116" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>137</v>
-      </c>
-      <c r="B117" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>357</v>
-      </c>
-      <c r="B118" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>358</v>
-      </c>
-      <c r="B119" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>359</v>
-      </c>
-      <c r="B120" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>360</v>
-      </c>
-      <c r="B121" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>361</v>
-      </c>
-      <c r="B122" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>362</v>
-      </c>
-      <c r="B123" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>363</v>
-      </c>
-      <c r="B124" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>364</v>
-      </c>
-      <c r="B125" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>365</v>
-      </c>
-      <c r="B126" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>366</v>
-      </c>
-      <c r="B127" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>367</v>
-      </c>
-      <c r="B128" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>368</v>
-      </c>
-      <c r="B129" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>369</v>
-      </c>
-      <c r="B130" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>370</v>
-      </c>
-      <c r="B131" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>371</v>
-      </c>
-      <c r="B132" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>372</v>
-      </c>
-      <c r="B133" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>373</v>
-      </c>
-      <c r="B134" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>108</v>
-      </c>
-      <c r="B135" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>374</v>
-      </c>
-      <c r="B136" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>375</v>
-      </c>
-      <c r="B137" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>376</v>
-      </c>
-      <c r="B138" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>377</v>
-      </c>
-      <c r="B139" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>378</v>
-      </c>
-      <c r="B140" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>379</v>
-      </c>
-      <c r="B141" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>380</v>
-      </c>
-      <c r="B142" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>381</v>
-      </c>
-      <c r="B143" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>382</v>
-      </c>
-      <c r="B144" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>383</v>
-      </c>
-      <c r="B145" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>384</v>
-      </c>
-      <c r="B146" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>385</v>
-      </c>
-      <c r="B147" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>386</v>
-      </c>
-      <c r="B148" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>387</v>
-      </c>
-      <c r="B149" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>388</v>
-      </c>
-      <c r="B150" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>389</v>
-      </c>
-      <c r="B151" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>390</v>
-      </c>
-      <c r="B152" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>391</v>
-      </c>
-      <c r="B153" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>392</v>
-      </c>
-      <c r="B154" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>393</v>
-      </c>
-      <c r="B155" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>108</v>
-      </c>
-      <c r="B156" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>374</v>
-      </c>
-      <c r="B157" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>394</v>
-      </c>
-      <c r="B158" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>376</v>
-      </c>
-      <c r="B159" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>395</v>
-      </c>
-      <c r="B160" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>396</v>
-      </c>
-      <c r="B161" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>397</v>
-      </c>
-      <c r="B162" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>102</v>
-      </c>
-      <c r="B163" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>398</v>
-      </c>
-      <c r="B164" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>399</v>
-      </c>
-      <c r="B165" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
-        <v>400</v>
-      </c>
-      <c r="B166" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>401</v>
-      </c>
-      <c r="B167" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>402</v>
-      </c>
-      <c r="B168" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>403</v>
-      </c>
-      <c r="B169" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>137</v>
-      </c>
-      <c r="B170" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
-        <v>357</v>
-      </c>
-      <c r="B171" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>404</v>
-      </c>
-      <c r="B172" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>405</v>
-      </c>
-      <c r="B173" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
-        <v>406</v>
-      </c>
-      <c r="B174" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
-        <v>378</v>
-      </c>
-      <c r="B175" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
-        <v>407</v>
-      </c>
-      <c r="B176" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
-        <v>408</v>
-      </c>
-      <c r="B177" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
-        <v>409</v>
-      </c>
-      <c r="B178" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
-        <v>410</v>
-      </c>
-      <c r="B179" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>411</v>
-      </c>
-      <c r="B180" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
-        <v>412</v>
-      </c>
-      <c r="B181" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
-        <v>413</v>
-      </c>
-      <c r="B182" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
-        <v>414</v>
-      </c>
-      <c r="B183" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
-        <v>137</v>
-      </c>
-      <c r="B184" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
-        <v>415</v>
-      </c>
-      <c r="B185" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>416</v>
-      </c>
-      <c r="B186" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>417</v>
-      </c>
-      <c r="B187" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>418</v>
-      </c>
-      <c r="B188" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
-        <v>419</v>
-      </c>
-      <c r="B189" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
-        <v>420</v>
-      </c>
-      <c r="B190" t="s">
-        <v>267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>